<commit_message>
menambahkan data kelas online
</commit_message>
<xml_diff>
--- a/public/database/DATA.xlsx
+++ b/public/database/DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKRIPSI\Project\timetable-schedule\public\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A740BF-1930-4133-A7D3-748700779F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D625D488-D0A2-42D8-A439-B7559D75B60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="950" activeTab="6" xr2:uid="{A45E902C-B954-4836-9532-7B18EBE736F7}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="366">
   <si>
     <t>subjectCode</t>
   </si>
@@ -1114,6 +1114,36 @@
   </si>
   <si>
     <t>17:00</t>
+  </si>
+  <si>
+    <t>ONLINE 1</t>
+  </si>
+  <si>
+    <t>ONLINE 2</t>
+  </si>
+  <si>
+    <t>ONLINE 3</t>
+  </si>
+  <si>
+    <t>ONLINE 4</t>
+  </si>
+  <si>
+    <t>ONLINE 5</t>
+  </si>
+  <si>
+    <t>ONLINE 6</t>
+  </si>
+  <si>
+    <t>ONLINE 7</t>
+  </si>
+  <si>
+    <t>ONLINE 8</t>
+  </si>
+  <si>
+    <t>ONLINE 9</t>
+  </si>
+  <si>
+    <t>ONLINE 10</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1156,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1304,6 +1334,12 @@
       <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1682,7 +1718,7 @@
     <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1732,6 +1768,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="24" builtinId="30" customBuiltin="1"/>
@@ -2220,8 +2259,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:F312"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F307" sqref="F307"/>
+    <sheetView topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="K314" sqref="K314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14411,13 +14450,16 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8258DD1C-5C89-4BF3-859D-C9EDC0429FAF}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="11" t="s">
@@ -14659,7 +14701,208 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:6" ht="15">
+      <c r="A13" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="B13" s="21">
+        <v>200</v>
+      </c>
+      <c r="C13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" s="21">
+        <v>200</v>
+      </c>
+      <c r="C14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15">
+      <c r="A15" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="B15" s="21">
+        <v>200</v>
+      </c>
+      <c r="C15" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="A16" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="B16" s="21">
+        <v>200</v>
+      </c>
+      <c r="C16" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15">
+      <c r="A17" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" s="21">
+        <v>200</v>
+      </c>
+      <c r="C17" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15">
+      <c r="A18" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" s="21">
+        <v>200</v>
+      </c>
+      <c r="C18" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15">
+      <c r="A19" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="B19" s="21">
+        <v>200</v>
+      </c>
+      <c r="C19" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B20" s="21">
+        <v>200</v>
+      </c>
+      <c r="C20" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15">
+      <c r="A21" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="B21" s="21">
+        <v>200</v>
+      </c>
+      <c r="C21" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15">
+      <c r="A22" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="B22" s="21">
+        <v>200</v>
+      </c>
+      <c r="C22" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
modified room capacity data
</commit_message>
<xml_diff>
--- a/public/database/DATA.xlsx
+++ b/public/database/DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKRIPSI\Project\timetable-schedule\public\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D625D488-D0A2-42D8-A439-B7559D75B60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C1859E-2258-4801-B825-B515D2A2EFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="950" activeTab="6" xr2:uid="{A45E902C-B954-4836-9532-7B18EBE736F7}"/>
   </bookViews>
@@ -2259,8 +2259,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:F312"/>
   <sheetViews>
-    <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="K314" sqref="K314"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14453,7 +14453,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14526,7 +14526,7 @@
         <v>245</v>
       </c>
       <c r="B4" s="12">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C4" s="20" t="b">
         <v>0</v>
@@ -14546,7 +14546,7 @@
         <v>246</v>
       </c>
       <c r="B5" s="12">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C5" s="20" t="b">
         <v>0</v>

</xml_diff>